<commit_message>
a little more spreadsheet clean up
</commit_message>
<xml_diff>
--- a/user_guide/data/Pooled_Funds_Task4_VE_Estimation.xlsx
+++ b/user_guide/data/Pooled_Funds_Task4_VE_Estimation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\VisionEval\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{36C0A460-BCE3-4029-AB96-79FF57EE0D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BDE8D4-BD0A-4A3E-9277-EBD803AE4227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FC5E4B6D-513C-486A-8409-7B34145AD233}"/>
   </bookViews>
@@ -2794,8 +2794,8 @@
   <dimension ref="A1:N125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <pane ySplit="5" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A124" sqref="A124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8098,13 +8098,13 @@
         <v>26</v>
       </c>
       <c r="I124" t="s">
-        <v>23</v>
+        <v>288</v>
       </c>
       <c r="J124" t="s">
         <v>519</v>
       </c>
       <c r="K124" t="s">
-        <v>23</v>
+        <v>517</v>
       </c>
       <c r="L124" t="s">
         <v>520</v>
@@ -8142,13 +8142,13 @@
         <v>26</v>
       </c>
       <c r="I125" t="s">
-        <v>23</v>
+        <v>288</v>
       </c>
       <c r="J125" t="s">
         <v>526</v>
       </c>
       <c r="K125" t="s">
-        <v>23</v>
+        <v>517</v>
       </c>
       <c r="L125" t="s">
         <v>527</v>
@@ -8454,12 +8454,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C18CD4DEF363E547BE01E072B5C8CADE" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="66fa1103ebadf93fb5c3fb7fd041298e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="91fe26aa-8303-4fe7-b35e-ec0a8764a6d3" xmlns:ns3="2497597c-adfd-4649-bd7b-d6fcec7c1097" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eb770262859f62bc96cef340afda770b" ns2:_="" ns3:_="">
     <xsd:import namespace="91fe26aa-8303-4fe7-b35e-ec0a8764a6d3"/>
@@ -8638,6 +8632,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -8648,23 +8648,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADADCF8F-7C06-488B-A5B5-CF819D6C6DC4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="91fe26aa-8303-4fe7-b35e-ec0a8764a6d3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="2497597c-adfd-4649-bd7b-d6fcec7c1097"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCFBCC8E-84E3-4FC9-AC5E-63E74349B4BD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8683,6 +8666,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADADCF8F-7C06-488B-A5B5-CF819D6C6DC4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="91fe26aa-8303-4fe7-b35e-ec0a8764a6d3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="2497597c-adfd-4649-bd7b-d6fcec7c1097"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07A176A9-2FBF-48AE-813D-7EBBDDB5C7A5}">
   <ds:schemaRefs>

</xml_diff>